<commit_message>
Linked Google Drive -1 26 02 25
Successfully enabled the user to load contents from Google Drive.
</commit_message>
<xml_diff>
--- a/Data/temp_filtered_data.xlsx
+++ b/Data/temp_filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
   <si>
     <t>Question</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>You can have up to 100 tables in a log.</t>
+  </si>
+  <si>
+    <t>20.</t>
+  </si>
+  <si>
+    <t>According to the document, you can create 250 curve shades.</t>
+  </si>
+  <si>
+    <t>According to the GEO application documentation, you can load up to 5 data files to form one curve.</t>
+  </si>
+  <si>
+    <t>According to the document, you can have 10000 symbols per plot.</t>
+  </si>
+  <si>
+    <t>According to the document, you can define up to 23 scales.</t>
   </si>
   <si>
     <t>100 tables can be presented in a log.</t>
@@ -476,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -513,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>0.7483487725257874</v>
@@ -533,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>0.6214057803153992</v>
@@ -553,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>0.9134054780006409</v>
@@ -573,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>0.7483487725257874</v>
@@ -593,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>0.8620253801345825</v>
@@ -613,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F7">
         <v>0.9348680973052979</v>
@@ -633,7 +648,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>0.7483487725257874</v>
@@ -653,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F9">
         <v>0.7252475619316101</v>
@@ -673,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F10">
         <v>0.9460949897766113</v>
@@ -693,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>0.8584091663360596</v>
@@ -713,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F12">
         <v>0.8710943460464478</v>
@@ -733,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F13">
         <v>0.8451892137527466</v>
@@ -753,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F14">
         <v>0.7252475619316101</v>
@@ -773,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F15">
         <v>0.9123421907424927</v>
@@ -793,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F16">
         <v>0.8799165487289429</v>
@@ -813,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F17">
         <v>0.8799165487289429</v>
@@ -833,10 +848,490 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F18">
         <v>0.8451892137527466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>59</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <v>0.230478972196579</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>0.230478972196579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21">
+        <v>0.9534614086151123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22">
+        <v>0.9534614086151123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23">
+        <v>0.647385835647583</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24">
+        <v>0.647385835647583</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25">
+        <v>0.8799165487289429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <v>0.8799165487289429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27">
+        <v>0.8716347217559814</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28">
+        <v>0.8716347217559814</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29">
+        <v>0.8617551922798157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30">
+        <v>0.8617551922798157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>0.230478972196579</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32">
+        <v>0.230478972196579</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33">
+        <v>0.9534614086151123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34">
+        <v>0.9534614086151123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>0.647385835647583</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36">
+        <v>0.647385835647583</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37">
+        <v>0.8799165487289429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38">
+        <v>0.8799165487289429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39">
+        <v>0.8716347217559814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40">
+        <v>0.8716347217559814</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41">
+        <v>0.9348680973052979</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="1">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42">
+        <v>0.9348680973052979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loaded More Relevant Responses -2
</commit_message>
<xml_diff>
--- a/Data/temp_filtered_data.xlsx
+++ b/Data/temp_filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Question</t>
   </si>
@@ -61,7 +61,13 @@
     <t>The maximum number of characters in a single text entry is 32000.</t>
   </si>
   <si>
+    <t>200 tracks can be defined in one ODF.</t>
+  </si>
+  <si>
     <t>450 curves can be loaded in one go.</t>
+  </si>
+  <si>
+    <t>250 / 32000 (varies per text type) are the maximum number of characters in a single text entry.</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>-0.01678333058953285</v>
+        <v>-0.02518575824797153</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -472,8 +478,11 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
       <c r="F3">
-        <v>0.005372118670493364</v>
+        <v>0.7644559144973755</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -490,7 +499,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>0.9253911972045898</v>
@@ -510,7 +519,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>0.9253911972045898</v>
@@ -529,8 +538,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
       <c r="F6">
-        <v>0.04994607716798782</v>
+        <v>0.913228452205658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ROUGE BLEU demo 27 02 25
Applied ROUGE & BLEU metrics for evaluating the quality of the generated responses.
</commit_message>
<xml_diff>
--- a/Data/temp_filtered_data.xlsx
+++ b/Data/temp_filtered_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Question</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>Expected Answer</t>
+  </si>
+  <si>
+    <t>BLEU_score</t>
+  </si>
+  <si>
+    <t>ROUGE_score</t>
   </si>
   <si>
     <t>similarity_score</t>
@@ -425,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,101 +453,137 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>-0.02518575824797153</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3">
+        <v>0.1207742128058413</v>
+      </c>
+      <c r="G3">
+        <v>0.2916666666666666</v>
+      </c>
+      <c r="H3">
         <v>0.7644559144973755</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4">
+        <v>6.373704167435469E-155</v>
+      </c>
+      <c r="G4">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="H4">
         <v>0.9253911972045898</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5">
+        <v>6.373704167435469E-155</v>
+      </c>
+      <c r="G5">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="H5">
         <v>0.9253911972045898</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6">
+        <v>0.3719426400061713</v>
+      </c>
+      <c r="G6">
+        <v>0.6896551724137931</v>
+      </c>
+      <c r="H6">
         <v>0.913228452205658</v>
       </c>
     </row>

</xml_diff>